<commit_message>
updated the optimizer excel file
</commit_message>
<xml_diff>
--- a/report/optimal_values_optimizer.xlsx
+++ b/report/optimal_values_optimizer.xlsx
@@ -6,13 +6,14 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="SIR" sheetId="1" r:id="rId4"/>
+    <sheet name="SEIR" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>Table 1</t>
   </si>
@@ -39,6 +40,15 @@
   </si>
   <si>
     <t>m=0 case</t>
+  </si>
+  <si>
+    <t>tau</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>E0</t>
   </si>
 </sst>
 </file>
@@ -72,7 +82,7 @@
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,6 +98,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="10"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -121,7 +137,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -146,6 +162,24 @@
     <xf numFmtId="59" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="2" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -165,6 +199,7 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="fff4f4f4"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1751,4 +1786,191 @@
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="C4" xSplit="2" ySplit="3" activePane="bottomRight" state="frozenSplit"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="0.25" style="8" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="8" customWidth="1"/>
+    <col min="3" max="3" width="12.25" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="8" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="8" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="8" customWidth="1"/>
+    <col min="7" max="7" width="12.25" style="8" customWidth="1"/>
+    <col min="8" max="8" width="12.25" style="8" customWidth="1"/>
+    <col min="9" max="256" width="12.25" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="2" customHeight="1"/>
+    <row r="2" ht="20.35" customHeight="1">
+      <c r="B2" s="3"/>
+      <c r="C2" t="s" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s" s="4">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s" s="4">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s" s="4">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s" s="4">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" ht="20.55" customHeight="1">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" ht="20.55" customHeight="1">
+      <c r="B4" t="s" s="5">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.311</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1.858</v>
+      </c>
+      <c r="E4" s="6">
+        <v>2.303</v>
+      </c>
+      <c r="F4" s="7">
+        <v>2.2e-06</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.171</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="5" ht="20.35" customHeight="1">
+      <c r="B5" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.839</v>
+      </c>
+      <c r="D5" s="9">
+        <v>3.524</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0.584</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2.1e-06</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0.112</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0.006</v>
+      </c>
+    </row>
+    <row r="6" ht="20.35" customHeight="1">
+      <c r="B6" t="s" s="5">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.352</v>
+      </c>
+      <c r="D6" s="6">
+        <v>2.174</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.702</v>
+      </c>
+      <c r="F6" s="7">
+        <v>2.4e-06</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.287</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.008</v>
+      </c>
+    </row>
+    <row r="7" ht="20.35" customHeight="1">
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8" ht="20.35" customHeight="1">
+      <c r="B8" s="11"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" ht="20.35" customHeight="1">
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+    </row>
+    <row r="10" ht="20.35" customHeight="1">
+      <c r="B10" s="11"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" ht="20.35" customHeight="1">
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+    </row>
+    <row r="12" ht="20.35" customHeight="1">
+      <c r="B12" s="11"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>